<commit_message>
feat: update the them_chung_chi_mau template file; replace with the latest version to ensure compliance with new standards
</commit_message>
<xml_diff>
--- a/public/templates/them_chung_chi_mau.xlsx
+++ b/public/templates/them_chung_chi_mau.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOANG\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A1E4B5-9E10-4935-93A7-0B90C4213044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EC5183-C6D9-49A9-8863-BEC7B1413FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Mã số sinh viên</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Số hiệu bằng</t>
-  </si>
-  <si>
-    <t>11/08/2025</t>
   </si>
   <si>
     <t>STT</t>
@@ -59,6 +56,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -132,6 +132,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -441,13 +447,14 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.08203125" style="3" customWidth="1"/>
-    <col min="2" max="3" width="15.58203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.58203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.58203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="19.9140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="15.58203125" style="3" customWidth="1"/>
@@ -455,16 +462,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -478,16 +485,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45870</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3">
         <v>12312313123</v>
@@ -498,16 +505,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45870</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3">
         <v>21212131231</v>

</xml_diff>